<commit_message>
Speed increase and efficency messurements
</commit_message>
<xml_diff>
--- a/messurements/Execution time.xlsx
+++ b/messurements/Execution time.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysiek/Documents/Studia/Programowanie_rownolegle/Laby/Zadanie4/messurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3283ED8C-59EB-924E-ADB7-9BE2C2FD3A14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8F1CE7-9E9D-C74C-BE55-EF9F6B76AA72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{0550A672-FDB1-1344-9BD4-6CE50F14B704}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>n</t>
   </si>
@@ -56,17 +56,20 @@
     <t>Parallel time [us]</t>
   </si>
   <si>
-    <t>Thread number</t>
-  </si>
-  <si>
     <t>n \ threads</t>
+  </si>
+  <si>
+    <t>Spped increase</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +90,13 @@
       <color rgb="FF000000"/>
       <name val="Fira Code Light"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,19 +115,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -429,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85730492-3075-6A42-BF72-DFFFAB3591B6}">
-  <dimension ref="B2:J13"/>
+  <dimension ref="B2:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="M24" activeCellId="1" sqref="B26:I29 M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,7 +508,7 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -515,9 +531,7 @@
       <c r="I10" s="1">
         <v>8</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" ht="17" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -597,10 +611,286 @@
         <v>331973</v>
       </c>
     </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1">
+        <v>7</v>
+      </c>
+      <c r="I18" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4">
+        <f>$C4/C11</f>
+        <v>1.9360155113911779</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" ref="D19:I19" si="0">$C4/D11</f>
+        <v>1.9100908656145386</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4858630952380953</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4513081395348837</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2386416498681967</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1452329749103942</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2856912924513118</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" ref="C20:I20" si="1">$C5/C12</f>
+        <v>3.393683143489743</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="1"/>
+        <v>3.731856849515987</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="1"/>
+        <v>4.036007740871165</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="1"/>
+        <v>3.7953162291169451</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="1"/>
+        <v>3.5860581801781488</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="1"/>
+        <v>2.7488980121002591</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="1"/>
+        <v>2.5825500903351535</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" ref="C21:I21" si="2">$C6/C13</f>
+        <v>5.1092489250015651</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="2"/>
+        <v>6.8827042425198819</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="2"/>
+        <v>7.8988197089864487</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="2"/>
+        <v>7.9623173625930894</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="2"/>
+        <v>8.3489310019340319</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="2"/>
+        <v>8.1145159376032492</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="2"/>
+        <v>7.6201257331168497</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1">
+        <v>5</v>
+      </c>
+      <c r="G26" s="1">
+        <v>6</v>
+      </c>
+      <c r="H26" s="1">
+        <v>7</v>
+      </c>
+      <c r="I26" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4">
+        <f>C19/C$18</f>
+        <v>0.96800775569558895</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" ref="D27:I27" si="3">D19/D$18</f>
+        <v>0.63669695520484615</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="3"/>
+        <v>0.37146577380952384</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="3"/>
+        <v>0.29026162790697674</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="3"/>
+        <v>0.20644027497803277</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="3"/>
+        <v>0.16360471070148488</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="3"/>
+        <v>0.16071141155641397</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" ref="C28:I28" si="4">C20/C$18</f>
+        <v>1.6968415717448715</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="4"/>
+        <v>1.2439522831719956</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="4"/>
+        <v>1.0090019352177912</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="4"/>
+        <v>0.75906324582338902</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="4"/>
+        <v>0.59767636336302477</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="4"/>
+        <v>0.39269971601432274</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="4"/>
+        <v>0.32281876129189419</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" ref="C29:I29" si="5">C21/C$18</f>
+        <v>2.5546244625007826</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="5"/>
+        <v>2.2942347475066271</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="5"/>
+        <v>1.9747049272466122</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="5"/>
+        <v>1.592463472518618</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" si="5"/>
+        <v>1.3914885003223387</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" si="5"/>
+        <v>1.1592165625147499</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" si="5"/>
+        <v>0.95251571663960621</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B25:I25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>